<commit_message>
moved to data folder
</commit_message>
<xml_diff>
--- a/data/Abovegound Belowground Biomass.xlsx
+++ b/data/Abovegound Belowground Biomass.xlsx
@@ -1,18 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\OneDrive\CAP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="149" documentId="11_C4B4BCF2F49868B440B5AF6F5D25536E65918A6A" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{AE184194-1691-4055-8EE5-B1E5D1FFD980}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2860" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="3260" yWindow="2860" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2011" sheetId="5" r:id="rId1"/>
     <sheet name="2012" sheetId="1" r:id="rId2"/>
     <sheet name="2013" sheetId="3" r:id="rId3"/>
+    <sheet name="2015" sheetId="6" r:id="rId4"/>
+    <sheet name="2016" sheetId="7" r:id="rId5"/>
+    <sheet name="2017" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -129,12 +144,57 @@
   </si>
   <si>
     <t>missing belowground</t>
+  </si>
+  <si>
+    <t>M4C</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>M1E</t>
+  </si>
+  <si>
+    <t>M1W</t>
+  </si>
+  <si>
+    <t>M4S</t>
+  </si>
+  <si>
+    <t>missing BG</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Std Dev</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M4N</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>missing AG</t>
+  </si>
+  <si>
+    <t>missing AG and BG</t>
+  </si>
+  <si>
+    <t>31-Nov-17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -368,6 +428,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -692,14 +760,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:B40"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
@@ -708,7 +776,7 @@
     <col min="11" max="11" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45">
+    <row r="1" spans="1:12" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -746,7 +814,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
         <v>40865</v>
       </c>
@@ -783,7 +851,7 @@
         <v>1.8731836195508587</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>40861</v>
       </c>
@@ -802,7 +870,7 @@
         <v>20.399999999999999</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G16" si="0">E3-F3</f>
+        <f t="shared" ref="G3:G14" si="0">E3-F3</f>
         <v>48.9</v>
       </c>
       <c r="H3">
@@ -814,15 +882,15 @@
         <v>20.100000000000001</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J15" si="1">H3-I3</f>
+        <f t="shared" ref="J3:J14" si="1">H3-I3</f>
         <v>118.20000000000002</v>
       </c>
       <c r="K3" s="5">
-        <f t="shared" ref="K3:K15" si="2">G3/J3</f>
+        <f t="shared" ref="K3:K14" si="2">G3/J3</f>
         <v>0.41370558375634509</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>40865</v>
       </c>
@@ -859,7 +927,7 @@
         <v>0.86129458388375169</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>40868</v>
       </c>
@@ -894,7 +962,7 @@
         <v>1.0124481327800829</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>40868</v>
       </c>
@@ -929,7 +997,7 @@
         <v>0.50988142292490113</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>40868</v>
       </c>
@@ -964,7 +1032,7 @@
         <v>0.61365235749472202</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>40875</v>
       </c>
@@ -1001,7 +1069,7 @@
         <v>0.73346178548490693</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>40875</v>
       </c>
@@ -1036,7 +1104,7 @@
         <v>0.84563758389261756</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>40875</v>
       </c>
@@ -1071,7 +1139,7 @@
         <v>1.22265625</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>40875</v>
       </c>
@@ -1109,7 +1177,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>40875</v>
       </c>
@@ -1144,7 +1212,7 @@
         <v>0.5280898876404494</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3">
         <v>40875</v>
       </c>
@@ -1181,7 +1249,7 @@
         <v>0.72007722007722008</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
         <v>40875</v>
       </c>
@@ -1216,15 +1284,15 @@
         <v>0.71647509578544066</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="18" spans="10:11">
+    <row r="18" spans="10:11" x14ac:dyDescent="0.55000000000000004">
       <c r="J18" t="s">
         <v>17</v>
       </c>
@@ -1233,7 +1301,7 @@
         <v>0.82267940753652724</v>
       </c>
     </row>
-    <row r="19" spans="10:11">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.55000000000000004">
       <c r="J19" t="s">
         <v>18</v>
       </c>
@@ -1254,14 +1322,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
@@ -1270,7 +1338,7 @@
     <col min="11" max="11" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45">
+    <row r="1" spans="1:11" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1305,7 +1373,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
         <v>41233</v>
       </c>
@@ -1340,7 +1408,7 @@
         <v>0.32245681381957775</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>41243</v>
       </c>
@@ -1378,7 +1446,7 @@
         <v>0.39585062240663899</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>41243</v>
       </c>
@@ -1417,7 +1485,7 @@
         <v>0.68019480519480524</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>41243</v>
       </c>
@@ -1459,7 +1527,7 @@
         <v>0.76064690026954163</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>41242</v>
       </c>
@@ -1501,7 +1569,7 @@
         <v>0.5584862385321101</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>41233</v>
       </c>
@@ -1540,7 +1608,7 @@
         <v>0.5093015093015093</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>41242</v>
       </c>
@@ -1582,7 +1650,7 @@
         <v>0.34889753566796361</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>41233</v>
       </c>
@@ -1621,7 +1689,7 @@
         <v>0.74569683509161588</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>41242</v>
       </c>
@@ -1663,7 +1731,7 @@
         <v>2.0584795321637426</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>41242</v>
       </c>
@@ -1705,7 +1773,7 @@
         <v>1.1745098039215687</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>41243</v>
       </c>
@@ -1747,7 +1815,7 @@
         <v>0.47884940778341789</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>41242</v>
       </c>
@@ -1789,7 +1857,7 @@
         <v>3.3764705882352941</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>41233</v>
       </c>
@@ -1831,7 +1899,7 @@
         <v>1.4335329341317367</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6">
         <v>41233</v>
       </c>
@@ -1873,7 +1941,7 @@
         <v>0.62919896640826878</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6">
         <v>41243</v>
       </c>
@@ -1912,7 +1980,7 @@
         <v>2.0894454382826475</v>
       </c>
     </row>
-    <row r="18" spans="10:11">
+    <row r="18" spans="10:11" x14ac:dyDescent="0.55000000000000004">
       <c r="J18" t="s">
         <v>17</v>
       </c>
@@ -1921,7 +1989,7 @@
         <v>1.0374678620806959</v>
       </c>
     </row>
-    <row r="19" spans="10:11">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.55000000000000004">
       <c r="J19" t="s">
         <v>18</v>
       </c>
@@ -1942,14 +2010,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
@@ -1958,7 +2026,7 @@
     <col min="11" max="11" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45">
+    <row r="1" spans="1:12" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1996,7 +2064,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
         <v>41579</v>
       </c>
@@ -2034,7 +2102,7 @@
         <v>0.23583344514513171</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>41579</v>
       </c>
@@ -2056,7 +2124,7 @@
         <v>11.51</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G15" si="0">E3-F3</f>
+        <f t="shared" ref="G3:G12" si="0">E3-F3</f>
         <v>136.38999999999999</v>
       </c>
       <c r="H3">
@@ -2068,15 +2136,15 @@
         <v>20.59</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J15" si="1">H3-I3</f>
+        <f t="shared" ref="J3:J12" si="1">H3-I3</f>
         <v>270.18</v>
       </c>
       <c r="K3" s="5">
-        <f t="shared" ref="K3:K15" si="2">G3/J3</f>
+        <f t="shared" ref="K3:K12" si="2">G3/J3</f>
         <v>0.50481160707676354</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>41579</v>
       </c>
@@ -2114,7 +2182,7 @@
         <v>1.4591897527554363</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>41579</v>
       </c>
@@ -2156,7 +2224,7 @@
         <v>0.61783439490445857</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>41579</v>
       </c>
@@ -2194,7 +2262,7 @@
         <v>1.7954199634814365</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>41579</v>
       </c>
@@ -2235,7 +2303,7 @@
         <v>0.52627547111996331</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>41579</v>
       </c>
@@ -2277,7 +2345,7 @@
         <v>1.2058038909493136</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>41579</v>
       </c>
@@ -2317,7 +2385,7 @@
         <v>0.93240217507196943</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>41579</v>
       </c>
@@ -2354,7 +2422,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>41579</v>
       </c>
@@ -2386,7 +2454,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>41579</v>
       </c>
@@ -2418,23 +2486,23 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="18" spans="10:11">
+    <row r="18" spans="10:11" x14ac:dyDescent="0.55000000000000004">
       <c r="J18" t="s">
         <v>17</v>
       </c>
@@ -2443,7 +2511,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="10:11">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.55000000000000004">
       <c r="J19" t="s">
         <v>18</v>
       </c>
@@ -2461,4 +2529,1175 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35FF3425-C125-416B-8E7C-8A0CFB2F6465}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="7.38671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2">
+        <v>42312</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2">
+        <f>29.7+27.8</f>
+        <v>57.5</v>
+      </c>
+      <c r="F2">
+        <v>20.9</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G10" si="0">E2-F2</f>
+        <v>36.6</v>
+      </c>
+      <c r="H2">
+        <v>119.3</v>
+      </c>
+      <c r="I2">
+        <v>11.1</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J10" si="1">H2-I2</f>
+        <v>108.2</v>
+      </c>
+      <c r="K2">
+        <f>G2/J2</f>
+        <v>0.33826247689463956</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2">
+        <v>42312</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3">
+        <v>49.6</v>
+      </c>
+      <c r="F3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>39.900000000000006</v>
+      </c>
+      <c r="H3">
+        <v>259.60000000000002</v>
+      </c>
+      <c r="I3">
+        <v>12.5</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="1"/>
+        <v>247.10000000000002</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K10" si="2">G3/J3</f>
+        <v>0.1614730878186969</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2">
+        <v>42312</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4">
+        <v>50.4</v>
+      </c>
+      <c r="F4">
+        <v>5.2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>45.199999999999996</v>
+      </c>
+      <c r="H4">
+        <f>120.2+192.3</f>
+        <v>312.5</v>
+      </c>
+      <c r="I4">
+        <f>11.2+9.6</f>
+        <v>20.799999999999997</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>291.7</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>0.15495371957490572</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2">
+        <v>42312</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <f>50.8+55.8</f>
+        <v>106.6</v>
+      </c>
+      <c r="F5">
+        <f>17+18.6</f>
+        <v>35.6</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="H5">
+        <f>102.9+244.3</f>
+        <v>347.20000000000005</v>
+      </c>
+      <c r="I5">
+        <f>19.7+24.7</f>
+        <v>44.4</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>302.80000000000007</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>0.23447820343461026</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2">
+        <v>42312</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <f>58.2+110.2</f>
+        <v>168.4</v>
+      </c>
+      <c r="F6">
+        <f>11.2+9.5</f>
+        <v>20.7</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>147.70000000000002</v>
+      </c>
+      <c r="H6">
+        <f>221.1+94.2</f>
+        <v>315.3</v>
+      </c>
+      <c r="I6">
+        <f>10.8+10.7</f>
+        <v>21.5</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>293.8</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>0.50272294077603819</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2">
+        <v>42312</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7">
+        <v>100.3</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>91.3</v>
+      </c>
+      <c r="H7">
+        <f>78.2+132.2+57.1</f>
+        <v>267.5</v>
+      </c>
+      <c r="I7">
+        <v>27.7</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>239.8</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>0.38073394495412843</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2">
+        <v>42313</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>61.2</v>
+      </c>
+      <c r="F8">
+        <v>10.8</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>50.400000000000006</v>
+      </c>
+      <c r="H8">
+        <v>194.1</v>
+      </c>
+      <c r="I8">
+        <v>10.5</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>183.6</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>0.27450980392156865</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2">
+        <v>42313</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <f>71.2+72.7</f>
+        <v>143.9</v>
+      </c>
+      <c r="F9">
+        <v>20.8</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>123.10000000000001</v>
+      </c>
+      <c r="H9">
+        <f>111.2+162.8</f>
+        <v>274</v>
+      </c>
+      <c r="I9">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>239.3</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>0.51441704972837443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2">
+        <v>42313</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10">
+        <v>201.1</v>
+      </c>
+      <c r="F10">
+        <v>20.7</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>180.4</v>
+      </c>
+      <c r="H10">
+        <f>210.7+297.9</f>
+        <v>508.59999999999997</v>
+      </c>
+      <c r="I10">
+        <v>23.9</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>484.7</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>0.37218898287600582</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="5">
+        <f>AVERAGE(K2:K10)</f>
+        <v>0.32597113444210751</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="5">
+        <f>_xlfn.STDEV.P(K2:K10)</f>
+        <v>0.12443873305221823</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D80274-A42F-405F-AEA3-1B57A87CDD4E}">
+  <dimension ref="A1:L13"/>
+  <sheetViews>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="31.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2">
+        <v>42705</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>66.7</v>
+      </c>
+      <c r="F2">
+        <v>10.8</v>
+      </c>
+      <c r="G2">
+        <f>E2-F2</f>
+        <v>55.900000000000006</v>
+      </c>
+      <c r="H2">
+        <v>66.3</v>
+      </c>
+      <c r="I2">
+        <v>11.1</v>
+      </c>
+      <c r="J2">
+        <f>H2-I2</f>
+        <v>55.199999999999996</v>
+      </c>
+      <c r="K2">
+        <f>G2/J2</f>
+        <v>1.01268115942029</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2">
+        <v>42705</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>61.5</v>
+      </c>
+      <c r="F3">
+        <v>10.4</v>
+      </c>
+      <c r="G3">
+        <f>E3-F3</f>
+        <v>51.1</v>
+      </c>
+      <c r="H3">
+        <v>66.5</v>
+      </c>
+      <c r="I3">
+        <v>10.8</v>
+      </c>
+      <c r="J3">
+        <f>H3-I3</f>
+        <v>55.7</v>
+      </c>
+      <c r="K3">
+        <f>G3/J3</f>
+        <v>0.91741472172351879</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2">
+        <v>42705</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4">
+        <v>51.8</v>
+      </c>
+      <c r="F4">
+        <v>11.6</v>
+      </c>
+      <c r="G4">
+        <f>E4-F4</f>
+        <v>40.199999999999996</v>
+      </c>
+      <c r="H4">
+        <v>60.6</v>
+      </c>
+      <c r="I4">
+        <v>12.6</v>
+      </c>
+      <c r="J4">
+        <f>H4-I4</f>
+        <v>48</v>
+      </c>
+      <c r="K4">
+        <f>G4/J4</f>
+        <v>0.83749999999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2">
+        <v>42705</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>48.2</v>
+      </c>
+      <c r="F5">
+        <v>10.1</v>
+      </c>
+      <c r="G5">
+        <f>E5-F5</f>
+        <v>38.1</v>
+      </c>
+      <c r="H5">
+        <v>147.6</v>
+      </c>
+      <c r="I5">
+        <v>11</v>
+      </c>
+      <c r="J5">
+        <f>H5-I5</f>
+        <v>136.6</v>
+      </c>
+      <c r="K5">
+        <f>G5/J5</f>
+        <v>0.27891654465592974</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2">
+        <v>42705</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6">
+        <v>55.1</v>
+      </c>
+      <c r="F6">
+        <v>10.4</v>
+      </c>
+      <c r="G6">
+        <f>E6-F6</f>
+        <v>44.7</v>
+      </c>
+      <c r="H6">
+        <v>141.69999999999999</v>
+      </c>
+      <c r="I6">
+        <v>11.4</v>
+      </c>
+      <c r="J6">
+        <f>H6-I6</f>
+        <v>130.29999999999998</v>
+      </c>
+      <c r="K6">
+        <f>G6/J6</f>
+        <v>0.34305448963929402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2">
+        <v>42705</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7">
+        <v>56.9</v>
+      </c>
+      <c r="F7">
+        <v>10.9</v>
+      </c>
+      <c r="G7">
+        <f>E7-F7</f>
+        <v>46</v>
+      </c>
+      <c r="L7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2">
+        <v>42705</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2">
+        <v>42705</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>28.7</v>
+      </c>
+      <c r="F9">
+        <v>10.7</v>
+      </c>
+      <c r="G9">
+        <f>E9-F9</f>
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>168.8</v>
+      </c>
+      <c r="I9">
+        <v>13.7</v>
+      </c>
+      <c r="J9">
+        <f>H9-I9</f>
+        <v>155.10000000000002</v>
+      </c>
+      <c r="K9">
+        <f>G9/J9</f>
+        <v>0.11605415860735008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2">
+        <v>42705</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>58.8</v>
+      </c>
+      <c r="F10">
+        <v>11.6</v>
+      </c>
+      <c r="G10">
+        <f>E10-F10</f>
+        <v>47.199999999999996</v>
+      </c>
+      <c r="L10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J12" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12">
+        <f>AVERAGE(K2:K10)</f>
+        <v>0.58427017900773037</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13">
+        <f>_xlfn.STDEV.P(K2:K10)</f>
+        <v>0.34863990240362425</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L10">
+    <sortCondition ref="B2:B10"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F93F10-AFE5-4321-896F-E119CA59D1FC}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.609375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2">
+        <v>43060</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>58.2+74.2</f>
+        <v>132.4</v>
+      </c>
+      <c r="I2">
+        <f>11.1+11</f>
+        <v>22.1</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J10" si="0">H2-I2</f>
+        <v>110.30000000000001</v>
+      </c>
+      <c r="L2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="2">
+        <v>43060</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="F3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G3">
+        <f>E3-F3</f>
+        <v>68.2</v>
+      </c>
+      <c r="H3">
+        <v>88.2</v>
+      </c>
+      <c r="I3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K10" si="1">G3/J3</f>
+        <v>0.85250000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2">
+        <v>43060</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <v>95.6</v>
+      </c>
+      <c r="F4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="G4">
+        <f>E4-F4</f>
+        <v>75.5</v>
+      </c>
+      <c r="H4">
+        <v>149.4</v>
+      </c>
+      <c r="I4">
+        <v>11.5</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>137.9</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>0.54749818709209574</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2">
+        <v>43060</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5">
+        <f>25.9+28.8</f>
+        <v>54.7</v>
+      </c>
+      <c r="I5">
+        <f>13.1+10.8</f>
+        <v>23.9</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>30.800000000000004</v>
+      </c>
+      <c r="L5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="2">
+        <v>43060</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6">
+        <v>53.2</v>
+      </c>
+      <c r="F6">
+        <v>20.9</v>
+      </c>
+      <c r="G6">
+        <f>E6-F6</f>
+        <v>32.300000000000004</v>
+      </c>
+      <c r="H6">
+        <f>41.5+28.3</f>
+        <v>69.8</v>
+      </c>
+      <c r="I6">
+        <f>9.8+6.9</f>
+        <v>16.700000000000003</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>53.099999999999994</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>0.6082862523540491</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2">
+        <v>43060</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="I7">
+        <v>11.3</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>25.400000000000002</v>
+      </c>
+      <c r="L7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <f>9.6+50.8</f>
+        <v>60.4</v>
+      </c>
+      <c r="I8">
+        <f>5.3+6.4</f>
+        <v>11.7</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>48.7</v>
+      </c>
+      <c r="L8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2">
+        <v>43042</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9">
+        <v>138.6</v>
+      </c>
+      <c r="F9">
+        <v>22.1</v>
+      </c>
+      <c r="G9">
+        <f>E9-F9</f>
+        <v>116.5</v>
+      </c>
+      <c r="H9">
+        <v>166.2</v>
+      </c>
+      <c r="I9">
+        <v>11.3</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>154.89999999999998</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>0.752098127824403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2">
+        <v>43060</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10">
+        <v>89.7</v>
+      </c>
+      <c r="F10">
+        <v>25.7</v>
+      </c>
+      <c r="G10">
+        <f>E10-F10</f>
+        <v>64</v>
+      </c>
+      <c r="H10">
+        <f>179.2+95.9</f>
+        <v>275.10000000000002</v>
+      </c>
+      <c r="I10">
+        <f>8.8+14.4</f>
+        <v>23.200000000000003</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>251.90000000000003</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>0.25406907502977366</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13">
+        <f>AVERAGE(K2:K10)</f>
+        <v>0.6028903284600643</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="J14" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14">
+        <f>_xlfn.STDEV.P(K2:K10)</f>
+        <v>0.20461751033677511</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A8" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added missing 2016 and 2017 AG/BG data
filled in gaps for missing data for AG or BG (or both) values for 2016 and 2017 datasets.
</commit_message>
<xml_diff>
--- a/data/Abovegound Belowground Biomass.xlsx
+++ b/data/Abovegound Belowground Biomass.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\OneDrive\CAP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrissanchez/Documents/weel/tres rios/datasets/tr-soil-root-cores/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="11_C4B4BCF2F49868B440B5AF6F5D25536E65918A6A" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{AE184194-1691-4055-8EE5-B1E5D1FFD980}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2952EA11-93B5-D64D-8B9C-14AF8B5F0DF5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2860" windowWidth="25600" windowHeight="18380" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8820" yWindow="3260" windowWidth="30180" windowHeight="21620" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2011" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -164,9 +164,6 @@
     <t>M4S</t>
   </si>
   <si>
-    <t>missing BG</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
@@ -180,12 +177,6 @@
   </si>
   <si>
     <t>M5</t>
-  </si>
-  <si>
-    <t>missing AG</t>
-  </si>
-  <si>
-    <t>missing AG and BG</t>
   </si>
   <si>
     <t>31-Nov-17</t>
@@ -767,7 +758,7 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
@@ -776,7 +767,7 @@
     <col min="11" max="11" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -814,7 +805,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>40865</v>
       </c>
@@ -851,7 +842,7 @@
         <v>1.8731836195508587</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>40861</v>
       </c>
@@ -890,7 +881,7 @@
         <v>0.41370558375634509</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>40865</v>
       </c>
@@ -927,7 +918,7 @@
         <v>0.86129458388375169</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>40868</v>
       </c>
@@ -962,7 +953,7 @@
         <v>1.0124481327800829</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>40868</v>
       </c>
@@ -997,7 +988,7 @@
         <v>0.50988142292490113</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>40868</v>
       </c>
@@ -1032,7 +1023,7 @@
         <v>0.61365235749472202</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>40875</v>
       </c>
@@ -1069,7 +1060,7 @@
         <v>0.73346178548490693</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>40875</v>
       </c>
@@ -1104,7 +1095,7 @@
         <v>0.84563758389261756</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>40875</v>
       </c>
@@ -1139,7 +1130,7 @@
         <v>1.22265625</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>40875</v>
       </c>
@@ -1177,7 +1168,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>40875</v>
       </c>
@@ -1212,7 +1203,7 @@
         <v>0.5280898876404494</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>40875</v>
       </c>
@@ -1249,7 +1240,7 @@
         <v>0.72007722007722008</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>40875</v>
       </c>
@@ -1284,15 +1275,15 @@
         <v>0.71647509578544066</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="18" spans="10:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J18" t="s">
         <v>17</v>
       </c>
@@ -1301,7 +1292,7 @@
         <v>0.82267940753652724</v>
       </c>
     </row>
-    <row r="19" spans="10:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J19" t="s">
         <v>18</v>
       </c>
@@ -1329,7 +1320,7 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
@@ -1338,7 +1329,7 @@
     <col min="11" max="11" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1364,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>41233</v>
       </c>
@@ -1408,7 +1399,7 @@
         <v>0.32245681381957775</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>41243</v>
       </c>
@@ -1446,7 +1437,7 @@
         <v>0.39585062240663899</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>41243</v>
       </c>
@@ -1485,7 +1476,7 @@
         <v>0.68019480519480524</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>41243</v>
       </c>
@@ -1527,7 +1518,7 @@
         <v>0.76064690026954163</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>41242</v>
       </c>
@@ -1569,7 +1560,7 @@
         <v>0.5584862385321101</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>41233</v>
       </c>
@@ -1608,7 +1599,7 @@
         <v>0.5093015093015093</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>41242</v>
       </c>
@@ -1650,7 +1641,7 @@
         <v>0.34889753566796361</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>41233</v>
       </c>
@@ -1689,7 +1680,7 @@
         <v>0.74569683509161588</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>41242</v>
       </c>
@@ -1731,7 +1722,7 @@
         <v>2.0584795321637426</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>41242</v>
       </c>
@@ -1773,7 +1764,7 @@
         <v>1.1745098039215687</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>41243</v>
       </c>
@@ -1815,7 +1806,7 @@
         <v>0.47884940778341789</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>41242</v>
       </c>
@@ -1857,7 +1848,7 @@
         <v>3.3764705882352941</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>41233</v>
       </c>
@@ -1899,7 +1890,7 @@
         <v>1.4335329341317367</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>41233</v>
       </c>
@@ -1941,7 +1932,7 @@
         <v>0.62919896640826878</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>41243</v>
       </c>
@@ -1980,7 +1971,7 @@
         <v>2.0894454382826475</v>
       </c>
     </row>
-    <row r="18" spans="10:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J18" t="s">
         <v>17</v>
       </c>
@@ -1989,7 +1980,7 @@
         <v>1.0374678620806959</v>
       </c>
     </row>
-    <row r="19" spans="10:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J19" t="s">
         <v>18</v>
       </c>
@@ -2017,7 +2008,7 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
@@ -2026,7 +2017,7 @@
     <col min="11" max="11" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2064,7 +2055,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>41579</v>
       </c>
@@ -2102,7 +2093,7 @@
         <v>0.23583344514513171</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>41579</v>
       </c>
@@ -2144,7 +2135,7 @@
         <v>0.50481160707676354</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>41579</v>
       </c>
@@ -2182,7 +2173,7 @@
         <v>1.4591897527554363</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>41579</v>
       </c>
@@ -2224,7 +2215,7 @@
         <v>0.61783439490445857</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>41579</v>
       </c>
@@ -2262,7 +2253,7 @@
         <v>1.7954199634814365</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>41579</v>
       </c>
@@ -2303,7 +2294,7 @@
         <v>0.52627547111996331</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>41579</v>
       </c>
@@ -2345,7 +2336,7 @@
         <v>1.2058038909493136</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>41579</v>
       </c>
@@ -2385,7 +2376,7 @@
         <v>0.93240217507196943</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>41579</v>
       </c>
@@ -2422,7 +2413,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>41579</v>
       </c>
@@ -2454,7 +2445,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>41579</v>
       </c>
@@ -2486,23 +2477,23 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="K16" s="5"/>
     </row>
-    <row r="18" spans="10:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J18" t="s">
         <v>17</v>
       </c>
@@ -2511,7 +2502,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="10:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.2">
       <c r="J19" t="s">
         <v>18</v>
       </c>
@@ -2539,14 +2530,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="7.38671875" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2584,7 +2575,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42312</v>
       </c>
@@ -2623,7 +2614,7 @@
         <v>0.33826247689463956</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>42312</v>
       </c>
@@ -2661,7 +2652,7 @@
         <v>0.1614730878186969</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>42312</v>
       </c>
@@ -2701,7 +2692,7 @@
         <v>0.15495371957490572</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>42312</v>
       </c>
@@ -2743,7 +2734,7 @@
         <v>0.23447820343461026</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>42312</v>
       </c>
@@ -2785,7 +2776,7 @@
         <v>0.50272294077603819</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>42312</v>
       </c>
@@ -2824,7 +2815,7 @@
         <v>0.38073394495412843</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>42313</v>
       </c>
@@ -2862,7 +2853,7 @@
         <v>0.27450980392156865</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>42313</v>
       </c>
@@ -2902,7 +2893,7 @@
         <v>0.51441704972837443</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>42313</v>
       </c>
@@ -2941,7 +2932,7 @@
         <v>0.37218898287600582</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J13" t="s">
         <v>17</v>
       </c>
@@ -2950,7 +2941,7 @@
         <v>0.32597113444210751</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J14" t="s">
         <v>18</v>
       </c>
@@ -2968,16 +2959,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D80274-A42F-405F-AEA3-1B57A87CDD4E}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3015,7 +3006,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>42705</v>
       </c>
@@ -3025,6 +3016,9 @@
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
       <c r="E2">
         <v>66.7</v>
       </c>
@@ -3032,7 +3026,7 @@
         <v>10.8</v>
       </c>
       <c r="G2">
-        <f>E2-F2</f>
+        <f t="shared" ref="G2:G7" si="0">E2-F2</f>
         <v>55.900000000000006</v>
       </c>
       <c r="H2">
@@ -3050,7 +3044,7 @@
         <v>1.01268115942029</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>42705</v>
       </c>
@@ -3060,6 +3054,9 @@
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
       <c r="E3">
         <v>61.5</v>
       </c>
@@ -3067,7 +3064,7 @@
         <v>10.4</v>
       </c>
       <c r="G3">
-        <f>E3-F3</f>
+        <f t="shared" si="0"/>
         <v>51.1</v>
       </c>
       <c r="H3">
@@ -3085,7 +3082,7 @@
         <v>0.91741472172351879</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>42705</v>
       </c>
@@ -3105,7 +3102,7 @@
         <v>11.6</v>
       </c>
       <c r="G4">
-        <f>E4-F4</f>
+        <f t="shared" si="0"/>
         <v>40.199999999999996</v>
       </c>
       <c r="H4">
@@ -3123,7 +3120,7 @@
         <v>0.83749999999999991</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>42705</v>
       </c>
@@ -3133,6 +3130,9 @@
       <c r="C5">
         <v>1</v>
       </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
       <c r="E5">
         <v>48.2</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>10.1</v>
       </c>
       <c r="G5">
-        <f>E5-F5</f>
+        <f t="shared" si="0"/>
         <v>38.1</v>
       </c>
       <c r="H5">
@@ -3158,7 +3158,7 @@
         <v>0.27891654465592974</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>42705</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>10.4</v>
       </c>
       <c r="G6">
-        <f>E6-F6</f>
+        <f t="shared" si="0"/>
         <v>44.7</v>
       </c>
       <c r="H6">
@@ -3196,7 +3196,7 @@
         <v>0.34305448963929402</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>42705</v>
       </c>
@@ -3216,14 +3216,25 @@
         <v>10.9</v>
       </c>
       <c r="G7">
-        <f>E7-F7</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="L7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="H7">
+        <v>109.1</v>
+      </c>
+      <c r="I7">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J7">
+        <f>H7-I7</f>
+        <v>100.3</v>
+      </c>
+      <c r="K7">
+        <f>G7/J7</f>
+        <v>0.45862412761714855</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>42705</v>
       </c>
@@ -3233,11 +3244,35 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="L8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>45.8</v>
+      </c>
+      <c r="F8">
+        <v>14.8</v>
+      </c>
+      <c r="G8">
+        <f>E8-F8</f>
+        <v>30.999999999999996</v>
+      </c>
+      <c r="H8">
+        <v>229.9</v>
+      </c>
+      <c r="I8">
+        <v>18.2</v>
+      </c>
+      <c r="J8">
+        <f>H8-I8</f>
+        <v>211.70000000000002</v>
+      </c>
+      <c r="K8">
+        <f>G8/J8</f>
+        <v>0.14643363249881905</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>42705</v>
       </c>
@@ -3246,6 +3281,9 @@
       </c>
       <c r="C9">
         <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
       </c>
       <c r="E9">
         <v>28.7</v>
@@ -3272,7 +3310,7 @@
         <v>0.11605415860735008</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>42705</v>
       </c>
@@ -3281,6 +3319,9 @@
       </c>
       <c r="C10">
         <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
       </c>
       <c r="E10">
         <v>58.8</v>
@@ -3292,26 +3333,36 @@
         <f>E10-F10</f>
         <v>47.199999999999996</v>
       </c>
-      <c r="L10" t="s">
+      <c r="H10">
+        <v>244.9</v>
+      </c>
+      <c r="I10">
+        <v>15.8</v>
+      </c>
+      <c r="J10">
+        <v>229.1</v>
+      </c>
+      <c r="K10">
+        <f>G10/J10</f>
+        <v>0.20602357049323439</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="J12" t="s">
-        <v>43</v>
       </c>
       <c r="K12">
         <f>AVERAGE(K2:K10)</f>
-        <v>0.58427017900773037</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.4796336005172871</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K13">
         <f>_xlfn.STDEV.P(K2:K10)</f>
-        <v>0.34863990240362425</v>
+        <v>0.33020492556491604</v>
       </c>
     </row>
   </sheetData>
@@ -3326,17 +3377,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F93F10-AFE5-4321-896F-E119CA59D1FC}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.609375" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3374,7 +3425,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43060</v>
       </c>
@@ -3383,6 +3434,19 @@
       </c>
       <c r="C2">
         <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2">
+        <v>86.7</v>
+      </c>
+      <c r="F2">
+        <v>10.1</v>
+      </c>
+      <c r="G2">
+        <f>E2-F2</f>
+        <v>76.600000000000009</v>
       </c>
       <c r="H2">
         <f>58.2+74.2</f>
@@ -3396,11 +3460,11 @@
         <f t="shared" ref="J2:J10" si="0">H2-I2</f>
         <v>110.30000000000001</v>
       </c>
-      <c r="L2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="K2">
+        <v>0.68549000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43060</v>
       </c>
@@ -3411,7 +3475,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3">
         <v>76.900000000000006</v>
@@ -3434,11 +3498,11 @@
         <v>80</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K10" si="1">G3/J3</f>
+        <f t="shared" ref="K2:K10" si="1">G3/J3</f>
         <v>0.85250000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43060</v>
       </c>
@@ -3449,7 +3513,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4">
         <v>95.6</v>
@@ -3476,7 +3540,7 @@
         <v>0.54749818709209574</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43060</v>
       </c>
@@ -3487,7 +3551,17 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>39.6</v>
+      </c>
+      <c r="F5">
+        <v>22.3</v>
+      </c>
+      <c r="G5">
+        <f>E5-F5</f>
+        <v>17.3</v>
       </c>
       <c r="H5">
         <f>25.9+28.8</f>
@@ -3501,11 +3575,11 @@
         <f t="shared" si="0"/>
         <v>30.800000000000004</v>
       </c>
-      <c r="L5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="K5">
+        <v>0.55897459999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43060</v>
       </c>
@@ -3516,7 +3590,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6">
         <v>53.2</v>
@@ -3545,7 +3619,7 @@
         <v>0.6082862523540491</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43060</v>
       </c>
@@ -3558,6 +3632,16 @@
       <c r="D7" t="s">
         <v>38</v>
       </c>
+      <c r="E7">
+        <v>34.1</v>
+      </c>
+      <c r="F7">
+        <v>19.2</v>
+      </c>
+      <c r="G7">
+        <f>E7-F7</f>
+        <v>14.900000000000002</v>
+      </c>
       <c r="H7">
         <v>36.700000000000003</v>
       </c>
@@ -3568,19 +3652,33 @@
         <f t="shared" si="0"/>
         <v>25.400000000000002</v>
       </c>
-      <c r="L7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>0.58661417322834652</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8">
         <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8">
+        <v>59.3</v>
+      </c>
+      <c r="F8">
+        <v>21.7</v>
+      </c>
+      <c r="G8">
+        <f>E8-F8</f>
+        <v>37.599999999999994</v>
       </c>
       <c r="H8">
         <f>9.6+50.8</f>
@@ -3594,11 +3692,12 @@
         <f t="shared" si="0"/>
         <v>48.7</v>
       </c>
-      <c r="L8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0.77207392197125235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43042</v>
       </c>
@@ -3609,7 +3708,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9">
         <v>138.6</v>
@@ -3632,11 +3731,11 @@
         <v>154.89999999999998</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f>G9/J9</f>
         <v>0.752098127824403</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>43060</v>
       </c>
@@ -3647,7 +3746,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10">
         <v>89.7</v>
@@ -3676,22 +3775,22 @@
         <v>0.25406907502977366</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K13">
         <f>AVERAGE(K2:K10)</f>
-        <v>0.6028903284600643</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.6241782597222133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K14">
         <f>_xlfn.STDEV.P(K2:K10)</f>
-        <v>0.20461751033677511</v>
+        <v>0.16428374573431484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>